<commit_message>
updated the Python models
</commit_message>
<xml_diff>
--- a/COVID-19.xlsx
+++ b/COVID-19.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timothycomeau/Dropbox/Covid-19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF207CB6-0680-2F41-9541-ECF328F092BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64F9FC3F-A0A1-BF46-A8CE-48B2CDBC6D32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7120" yWindow="5420" windowWidth="28400" windowHeight="14820" firstSheet="1" activeTab="9" xr2:uid="{A5CB126D-F2C1-CC4E-886A-16083F7D0908}"/>
+    <workbookView xWindow="6500" yWindow="2220" windowWidth="28400" windowHeight="14820" firstSheet="2" activeTab="5" xr2:uid="{A5CB126D-F2C1-CC4E-886A-16083F7D0908}"/>
   </bookViews>
   <sheets>
     <sheet name="World" sheetId="1" r:id="rId1"/>
@@ -20013,7 +20013,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B15537FA-A914-8447-94D5-3E0CD69DDCA2}">
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J45" sqref="J45"/>
     </sheetView>
   </sheetViews>
@@ -23338,8 +23338,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5A86A38-08EC-FA44-A810-5EDDE230B175}">
   <dimension ref="A1:BE28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AI28" sqref="AI28"/>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="AI1" sqref="AI1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23450,7 +23450,7 @@
       <c r="AH1" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="AI1" s="37" t="s">
+      <c r="AI1" s="1" t="s">
         <v>70</v>
       </c>
       <c r="AJ1" s="1" t="s">
@@ -30389,8 +30389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C248010-6C16-954B-BC86-379C97BD27B4}">
   <dimension ref="A1:AY128"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="AX30" sqref="AX30"/>
+    <sheetView topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -44376,9 +44376,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82FE7191-96E7-3B4B-B5CF-F14CB9DCB66F}">
   <dimension ref="A1:AW133"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AR74" sqref="AR74"/>
+      <selection pane="bottomLeft" activeCell="B87" sqref="B87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -56468,9 +56468,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCA40CCA-C389-C042-8A50-528E4E4EFC4E}">
   <dimension ref="A1:AC140"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AC85" sqref="AC85"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:B84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>